<commit_message>
Available area re-parametrized, membrane sheet updated with the new parameter
</commit_message>
<xml_diff>
--- a/Data/Surface_growth_rate_data/surface_mumax.xlsx
+++ b/Data/Surface_growth_rate_data/surface_mumax.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\claud\Documents\PAModelpy_\Data\Surface_growth_rate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D517718-B978-495E-AF1A-BE158D91416C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A0A1D1-778B-4FC4-966C-4B1C5E5055E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>A_occupied [um2/um2]</t>
+    <t>mumax [1/h]</t>
   </si>
   <si>
-    <t>mumax [1/h]</t>
+    <t>A_available [um2]</t>
   </si>
 </sst>
 </file>
@@ -240,13 +251,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.49</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.51</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -258,13 +269,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9.5413700000000004E-2</c:v>
+                  <c:v>17.133747433770118</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6594319999999997E-2</c:v>
+                  <c:v>7.263647061624285</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.7054538400000006E-2</c:v>
+                  <c:v>5.5882381175340434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1436,45 +1447,45 @@
   <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1.9</v>
+      </c>
+      <c r="B3">
+        <v>17.133747433770118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0.82</v>
+      </c>
+      <c r="B4">
+        <v>7.263647061624285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>0.49</v>
       </c>
-      <c r="B3">
-        <v>9.5413700000000004E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>0.51</v>
-      </c>
-      <c r="B4">
-        <v>9.6594319999999997E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>0.57999999999999996</v>
-      </c>
       <c r="B5">
-        <v>8.7054538400000006E-2</v>
+        <v>5.5882381175340434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>